<commit_message>
feat: add script to obtain the interface; add the site classification
</commit_message>
<xml_diff>
--- a/data collection of PDB/data/YCL040W_site_definition.xlsx
+++ b/data collection of PDB/data/YCL040W_site_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luho/PycharmProjects/3D_model/evolution/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA376F1-D3B3-5541-AB31-A8F92515C683}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657BBC39-DFFB-C145-9879-52CF6C7F1DDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37360" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9420" yWindow="8000" windowWidth="37360" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_site" sheetId="1" r:id="rId1"/>
@@ -1131,16 +1131,16 @@
   <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C1" sqref="C1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="5" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -1364,12 +1364,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>